<commit_message>
Ajustes no FPA e adicionando casos de teste
</commit_message>
<xml_diff>
--- a/3SI_GS_2/Governanca/FerramentaFPA-ProfRJP-Automatica-HEALTHTIE.xlsx
+++ b/3SI_GS_2/Governanca/FerramentaFPA-ProfRJP-Automatica-HEALTHTIE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codigos\Git\FIAP_3SI\3SI_GS_2\Governanca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D768C276-46B7-45B2-A9AE-CA39CC28BD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C9A4A4-DB59-44A1-AE81-0368866C9598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18735" windowHeight="16200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18735" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pontos Nao Ajustados" sheetId="1" r:id="rId1"/>
@@ -1641,8 +1641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N424"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N247" sqref="N247"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,7 +1780,7 @@
       </c>
       <c r="E12" s="47"/>
       <c r="F12" s="29">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G12" s="39" t="str">
         <f t="shared" ref="G12:G75" si="1">IF(OR(AND(B12="EE",D12&lt;2,F12&lt;16),AND(B12="EE",D12&lt;3,F12&lt;5),AND(B12="CE",D12&lt;2,F12&lt;20),AND(B12="CE",D12&lt;4,F12&lt;6),AND(B12="ALI",D12&lt;2,F12&lt;51),AND(B12="ALI",D12&lt;6,F12&lt;20),AND(B12="AIE",D12&lt;2,F12&lt;51),AND(B12="AIE",D12&lt;6,F12&lt;20)),"Simples",IF(OR(AND(B12="EE",D12=2,F12&gt;15),AND(B12="EE",D12&gt;2,F12&gt;4),AND(B12="CE",AND(D12&gt;1,D12&lt;4),F12&gt;19),AND(B12="CE",D12&gt;3,F12&gt;5),AND(B12="ALI",AND(D12&gt;1,D12&lt;6),F12&gt;50),AND(B12="ALI",D12&gt;5,F12&gt;19),AND(B12="AIE",AND(D12&gt;1,D12&lt;6),F12&gt;50),AND(B12="AIE",D12&gt;5,F12&gt;19)),"Complexo",IF(OR(B12="",D12="",F12=""),"","Medio")))</f>
@@ -2068,7 +2068,7 @@
       </c>
       <c r="E24" s="31"/>
       <c r="F24" s="32">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G24" s="39" t="str">
         <f t="shared" si="1"/>
@@ -2092,7 +2092,7 @@
       </c>
       <c r="E25" s="31"/>
       <c r="F25" s="32">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G25" s="39" t="str">
         <f t="shared" si="1"/>
@@ -2356,7 +2356,7 @@
       </c>
       <c r="E36" s="31"/>
       <c r="F36" s="32">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G36" s="39" t="str">
         <f t="shared" si="1"/>
@@ -2692,7 +2692,7 @@
       </c>
       <c r="E50" s="31"/>
       <c r="F50" s="32">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G50" s="39" t="str">
         <f t="shared" si="1"/>
@@ -11268,8 +11268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>